<commit_message>
adjust scar16 barrel and base
</commit_message>
<xml_diff>
--- a/changes/556-barrels.xlsx
+++ b/changes/556-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FB9E93-EE16-4B08-A551-EFFA52696D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8914DF35-569E-4EDE-A40E-C35B650993AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,16 +2312,16 @@
         <v>72</v>
       </c>
       <c r="C24">
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="D24">
         <v>0.73</v>
       </c>
       <c r="E24">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="F24">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="H24">
         <v>-0.1</v>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="N24" s="1">
         <f>C24-D24*20-E24*0.8-F24*0.6-H24*5+I24*10+J24/300</f>
-        <v>-12.033333333333335</v>
+        <v>-12.233333333333336</v>
       </c>
       <c r="P24">
         <v>0.14000000000000001</v>

</xml_diff>

<commit_message>
add aug 18 incher
</commit_message>
<xml_diff>
--- a/changes/556-barrels.xlsx
+++ b/changes/556-barrels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8914DF35-569E-4EDE-A40E-C35B650993AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55CBA7A-37E3-4EB6-A79E-C03F80F27BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>new</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>Steyr AUG HBAR 5.56x45 620mm Heavy LMG</t>
+  </si>
+  <si>
+    <t>steyr_aug_457mm_barrel</t>
+  </si>
+  <si>
+    <t>Steyr AUG A3 5.56x45 457mm</t>
   </si>
 </sst>
 </file>
@@ -1117,18 +1123,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X38"/>
+  <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="22" width="6.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1146,7 +1153,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1263,7 +1270,7 @@
         <v>2099.6999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1300,7 +1307,7 @@
         <v>1600</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" ref="N4:N35" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
+        <f t="shared" ref="N4:N36" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+I4*10+J4/300</f>
         <v>-6.9766666666666675</v>
       </c>
       <c r="P4">
@@ -1310,7 +1317,7 @@
         <v>20</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S31" si="1">ROUND(Q4*0.033+P4+R4, 2)</f>
+        <f t="shared" ref="S4:S32" si="1">ROUND(Q4*0.033+P4+R4, 2)</f>
         <v>0.84</v>
       </c>
       <c r="U4">
@@ -1325,7 +1332,7 @@
         <v>0.80952380952380965</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1386,7 +1393,7 @@
         <v>2099.94</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1447,7 +1454,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1505,7 +1512,7 @@
         <v>1979.94</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1564,7 +1571,7 @@
         <v>1679.94</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1623,7 +1630,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1676,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1730,7 +1737,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1786,7 +1793,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1842,7 +1849,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1898,7 +1905,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1953,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -2011,7 +2018,7 @@
         <v>899.69999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2066,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2089,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2138,7 +2145,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -2190,7 +2197,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -2242,7 +2249,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
@@ -2294,7 +2301,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2304,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2396,7 +2403,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2452,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2466,13 +2473,13 @@
         <v>0.99</v>
       </c>
       <c r="E28">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F28">
         <v>-7</v>
       </c>
       <c r="H28">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I28">
         <v>0.32</v>
@@ -2485,7 +2492,7 @@
       </c>
       <c r="N28" s="1">
         <f>C28-D28*20-E28*0.8-F28*0.6-H28*5+I28*10+J28/300</f>
-        <v>-17.400000000000002</v>
+        <v>-16.100000000000001</v>
       </c>
       <c r="P28">
         <v>0.1</v>
@@ -2501,7 +2508,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2509,19 +2516,19 @@
         <v>76</v>
       </c>
       <c r="C29">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="D29">
         <v>0.76</v>
       </c>
       <c r="E29">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="F29">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="H29">
-        <v>-0.1</v>
+        <v>-0.15</v>
       </c>
       <c r="I29">
         <v>0.24</v>
@@ -2534,7 +2541,7 @@
       </c>
       <c r="N29" s="1">
         <f>C29-D29*20-E29*0.8-F29*0.6-H29*5+I29*10+J29/300</f>
-        <v>-10.733333333333331</v>
+        <v>-10.08333333333333</v>
       </c>
       <c r="P29">
         <v>0.1</v>
@@ -2547,246 +2554,293 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="D30">
-        <v>0.63</v>
+        <v>0.69</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>-0.08</v>
       </c>
       <c r="I30">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="J30">
-        <v>150</v>
+        <v>275</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" si="0"/>
-        <v>-11.1</v>
+        <f t="shared" ref="N30:N31" si="3">C30-D30*20-E30*0.8-F30*0.6-H30*5+I30*10+J30/300</f>
+        <v>-10.083333333333334</v>
       </c>
       <c r="P30">
         <v>0.1</v>
       </c>
       <c r="Q30">
-        <v>16.023599999999998</v>
+        <v>17.992100000000001</v>
       </c>
       <c r="S30">
         <f t="shared" si="1"/>
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>0.55000000000000004</v>
-      </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
         <v>0.1</v>
       </c>
-      <c r="I31">
-        <v>-0.04</v>
-      </c>
       <c r="J31">
-        <v>-50</v>
+        <v>150</v>
       </c>
       <c r="M31">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" si="0"/>
-        <v>-11.466666666666667</v>
+        <f t="shared" si="3"/>
+        <v>-11.1</v>
       </c>
       <c r="P31">
         <v>0.1</v>
       </c>
       <c r="Q31">
-        <v>13.779500000000001</v>
+        <v>16.023599999999998</v>
       </c>
       <c r="S31">
         <f t="shared" si="1"/>
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0.1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>-50</v>
+      </c>
+      <c r="M32">
+        <v>600</v>
+      </c>
       <c r="N32" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33">
-        <v>-1</v>
-      </c>
-      <c r="D33">
-        <v>0.08</v>
-      </c>
-      <c r="E33">
-        <v>-2</v>
-      </c>
-      <c r="F33">
-        <v>-2</v>
-      </c>
-      <c r="M33">
-        <v>750</v>
-      </c>
+        <v>-10.466666666666667</v>
+      </c>
+      <c r="P32">
+        <v>0.1</v>
+      </c>
+      <c r="Q32">
+        <v>13.779500000000001</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N33" s="1">
         <f t="shared" si="0"/>
-        <v>0.19999999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D34">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="E34">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F34">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M34">
-        <v>1200</v>
+        <v>750</v>
       </c>
       <c r="N34" s="1">
         <f t="shared" si="0"/>
-        <v>0.20000000000000007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F35">
         <v>-1</v>
       </c>
       <c r="M35">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="N35" s="1">
         <f t="shared" si="0"/>
+        <v>0.20000000000000007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>-1</v>
+      </c>
+      <c r="M36">
+        <v>1000</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" si="0"/>
         <v>-1.4</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="C36">
+      <c r="C37">
         <v>3</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>0.11</v>
       </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <v>0</v>
-      </c>
-      <c r="N36" s="1">
-        <f>C36-D36*20-E36*0.8-F36*0.6-H36*5+I36*10+J36/300</f>
-        <v>0.79999999999999982</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
       <c r="N37" s="1">
         <f>C37-D37*20-E37*0.8-F37*0.6-H37*5+I37*10+J37/300</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38">
-        <v>-1</v>
-      </c>
-      <c r="D38">
-        <v>0.09</v>
-      </c>
-      <c r="E38">
-        <v>-3</v>
-      </c>
-      <c r="F38">
-        <v>-2</v>
-      </c>
-      <c r="M38">
-        <v>0</v>
-      </c>
+        <v>0.79999999999999982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="N38" s="1">
         <f>C38-D38*20-E38*0.8-F38*0.6-H38*5+I38*10+J38/300</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>-1</v>
+      </c>
+      <c r="D39">
+        <v>0.09</v>
+      </c>
+      <c r="E39">
+        <v>-3</v>
+      </c>
+      <c r="F39">
+        <v>-2</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <f>C39-D39*20-E39*0.8-F39*0.6-H39*5+I39*10+J39/300</f>
         <v>0.80000000000000049</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buff shorter 5.56 barrels a little
</commit_message>
<xml_diff>
--- a/changes/556-barrels.xlsx
+++ b/changes/556-barrels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55CBA7A-37E3-4EB6-A79E-C03F80F27BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A322698-8EBD-4655-870F-6BF6B81B9854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="m4-barrels" sheetId="1" r:id="rId1"/>
@@ -1125,17 +1125,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
-    <col min="3" max="22" width="6.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="22" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1153,7 +1153,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>2099.6999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>0.80952380952380965</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>2099.94</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>2232</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1979.94</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>1679.94</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>2094</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>0.62</v>
       </c>
       <c r="E11" s="1">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="F11" s="1">
         <v>-4</v>
@@ -1707,7 +1707,7 @@
         <v>0.1</v>
       </c>
       <c r="I11" s="1">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="J11" s="1">
         <v>-70</v>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
-        <v>-5.1333333333333329</v>
+        <v>-5.833333333333333</v>
       </c>
       <c r="P11">
         <v>0.15</v>
@@ -1737,7 +1737,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>0.15</v>
       </c>
       <c r="I12" s="1">
-        <v>-0.06</v>
+        <v>-0.04</v>
       </c>
       <c r="J12" s="1">
         <v>-117</v>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1400000000000006</v>
+        <v>-6.9400000000000013</v>
       </c>
       <c r="P12">
         <v>0.12</v>
@@ -1793,7 +1793,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>0.2</v>
       </c>
       <c r="I13" s="1">
-        <v>-0.1</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="J13" s="1">
         <v>-178</v>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
-        <v>-7.1933333333333342</v>
+        <v>-6.8933333333333344</v>
       </c>
       <c r="P13">
         <v>0.12</v>
@@ -1849,7 +1849,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1863,17 +1863,17 @@
         <v>0.47</v>
       </c>
       <c r="E14" s="1">
+        <v>-2</v>
+      </c>
+      <c r="F14" s="1">
         <v>-1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>-2</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
         <v>0.25</v>
       </c>
       <c r="I14" s="1">
-        <v>-0.14000000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="J14" s="1">
         <v>-239</v>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="N14" s="1">
         <f t="shared" si="0"/>
-        <v>-7.8466666666666658</v>
+        <v>-7.2466666666666661</v>
       </c>
       <c r="P14">
         <v>0.12</v>
@@ -1905,7 +1905,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>0.4</v>
       </c>
       <c r="I15" s="1">
-        <v>-0.2</v>
+        <v>-0.16</v>
       </c>
       <c r="J15" s="1">
         <v>-633</v>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>-8.31</v>
+        <v>-7.91</v>
       </c>
       <c r="P15">
         <v>0.09</v>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0.6</v>
       </c>
       <c r="I16" s="1">
-        <v>-0.26</v>
+        <v>-0.24</v>
       </c>
       <c r="J16" s="1">
         <v>-685</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-9.0833333333333321</v>
+        <v>-8.8833333333333329</v>
       </c>
       <c r="P16">
         <v>7.0000000000000007E-2</v>
@@ -2018,7 +2018,7 @@
         <v>899.69999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>0.2</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.12</v>
+        <v>-0.05</v>
       </c>
       <c r="J21" s="1">
         <v>-220</v>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="N21" s="1">
         <f>C21-D21*20-E21*0.8-F21*0.6-H21*5+I21*10+J21/300</f>
-        <v>-16.733333333333331</v>
+        <v>-16.033333333333331</v>
       </c>
       <c r="P21">
         <v>0.14000000000000001</v>
@@ -2249,7 +2249,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>0.2</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.13</v>
+        <v>-0.1</v>
       </c>
       <c r="J22" s="1">
         <v>-240</v>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>-17.3</v>
+        <v>-17</v>
       </c>
       <c r="P22">
         <v>0.14000000000000001</v>
@@ -2301,7 +2301,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N23" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>0.2</v>
       </c>
       <c r="I26">
-        <v>-0.12</v>
+        <v>-0.08</v>
       </c>
       <c r="J26">
         <v>-250</v>
@@ -2436,7 +2436,7 @@
       </c>
       <c r="N26" s="1">
         <f t="shared" si="0"/>
-        <v>-12.433333333333332</v>
+        <v>-12.033333333333333</v>
       </c>
       <c r="P26">
         <v>0.14000000000000001</v>
@@ -2449,7 +2449,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="N27" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2692,13 +2692,13 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N33" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>0.20000000000000007</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>-1.4</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
@@ -2806,13 +2806,13 @@
         <v>0.79999999999999982</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N38" s="1">
         <f>C38-D38*20-E38*0.8-F38*0.6-H38*5+I38*10+J38/300</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
slight 556 short barrel adjustment
</commit_message>
<xml_diff>
--- a/changes/556-barrels.xlsx
+++ b/changes/556-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A322698-8EBD-4655-870F-6BF6B81B9854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040AEC3A-C083-45F0-AC92-B13CC0C08502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,17 +1919,17 @@
         <v>0.34</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F15" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
         <v>0.4</v>
       </c>
       <c r="I15" s="1">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="J15" s="1">
         <v>-633</v>
@@ -1943,7 +1943,7 @@
       </c>
       <c r="N15" s="1">
         <f t="shared" si="0"/>
-        <v>-7.91</v>
+        <v>-7.6100000000000012</v>
       </c>
       <c r="P15">
         <v>0.09</v>
@@ -1974,7 +1974,7 @@
         <v>0.24</v>
       </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1984,7 +1984,7 @@
         <v>0.6</v>
       </c>
       <c r="I16" s="1">
-        <v>-0.24</v>
+        <v>-0.2</v>
       </c>
       <c r="J16" s="1">
         <v>-685</v>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="N16" s="1">
         <f t="shared" si="0"/>
-        <v>-8.8833333333333329</v>
+        <v>-7.6833333333333336</v>
       </c>
       <c r="P16">
         <v>7.0000000000000007E-2</v>

</xml_diff>

<commit_message>
fix hk barrels with irons
</commit_message>
<xml_diff>
--- a/changes/556-barrels.xlsx
+++ b/changes/556-barrels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA6299F-2E5C-435E-BEF2-AEBD3686F173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228BA0E4-4240-435F-82BF-5E0E298CAEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="H15" sqref="H15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,7 +2104,7 @@
         <v>63</v>
       </c>
       <c r="C19">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="D19">
         <v>0.86</v>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="N19" s="1">
         <f>C19-D19*20-E19*0.8-F19*0.6-H19*5+I19*10+J19/300</f>
-        <v>-17.399999999999999</v>
+        <v>-18.399999999999999</v>
       </c>
       <c r="P19">
         <v>0.2</v>
@@ -2150,7 +2150,7 @@
         <v>61</v>
       </c>
       <c r="C20" s="1">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D20" s="1">
         <v>0.68</v>
@@ -2178,7 +2178,7 @@
       </c>
       <c r="N20" s="1">
         <f>C20-D20*20-E20*0.8-F20*0.6-H20*5+I20*10+J20/300</f>
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="P20">
         <v>0.2</v>
@@ -2215,7 +2215,7 @@
         <v>0.2</v>
       </c>
       <c r="I21" s="1">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="J21" s="1">
         <v>-220</v>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="N21" s="1">
         <f>C21-D21*20-E21*0.8-F21*0.6-H21*5+I21*10+J21/300</f>
-        <v>-17.033333333333339</v>
+        <v>-17.133333333333336</v>
       </c>
       <c r="P21">
         <v>0.2</v>
@@ -2257,14 +2257,14 @@
         <v>4</v>
       </c>
       <c r="F22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1">
         <v>0.2</v>
       </c>
       <c r="I22" s="1">
-        <v>-0.1</v>
+        <v>-0.08</v>
       </c>
       <c r="J22" s="1">
         <v>-240</v>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="N22" s="1">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-17.2</v>
       </c>
       <c r="P22">
         <v>0.2</v>

</xml_diff>